<commit_message>
Naive model comparison added
</commit_message>
<xml_diff>
--- a/reports/evaluation.xlsx
+++ b/reports/evaluation.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Metrics by forecasted step" sheetId="1" r:id="rId1"/>
-    <sheet name="Metrics at each index" sheetId="2" r:id="rId2"/>
+    <sheet name="Naive forecast" sheetId="2" r:id="rId2"/>
+    <sheet name="Metrics at each index" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>RMSE</t>
   </si>
@@ -406,13 +407,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>128.2903801822572</v>
+        <v>131.7036362938518</v>
       </c>
       <c r="C2">
-        <v>91.89008810706966</v>
+        <v>83.61886512469947</v>
       </c>
       <c r="D2">
-        <v>126.029201705059</v>
+        <v>129.2584131052921</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -420,13 +421,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>112.4304805517197</v>
+        <v>117.7477190732956</v>
       </c>
       <c r="C3">
-        <v>82.82896458421435</v>
+        <v>72.82756226062774</v>
       </c>
       <c r="D3">
-        <v>107.8337799378804</v>
+        <v>104.6217378060333</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -434,13 +435,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.2231860420419853</v>
+        <v>0.2124154077354063</v>
       </c>
       <c r="C4">
-        <v>0.1591731801148343</v>
+        <v>0.1283451617272169</v>
       </c>
       <c r="D4">
-        <v>0.1946753984052607</v>
+        <v>0.1633663998056427</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -448,13 +449,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.2247287273334758</v>
+        <v>0.2257055770862675</v>
       </c>
       <c r="C5">
-        <v>0.1655491378721453</v>
+        <v>0.1308813749474227</v>
       </c>
       <c r="D5">
-        <v>0.2127955222951788</v>
+        <v>0.1845446686057443</v>
       </c>
     </row>
   </sheetData>
@@ -464,7 +465,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>131.7036362938518</v>
+      </c>
+      <c r="C2">
+        <v>83.61886512469947</v>
+      </c>
+      <c r="D2">
+        <v>129.2584131052921</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>117.7477190732956</v>
+      </c>
+      <c r="C3">
+        <v>72.82756226062774</v>
+      </c>
+      <c r="D3">
+        <v>104.6217378060333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.2124154077354063</v>
+      </c>
+      <c r="C4">
+        <v>0.1283451617272169</v>
+      </c>
+      <c r="D4">
+        <v>0.1633663998056427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.2257055770862675</v>
+      </c>
+      <c r="C5">
+        <v>0.1308813749474227</v>
+      </c>
+      <c r="D5">
+        <v>0.1845446686057443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -489,16 +570,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>77.5621785481771</v>
+        <v>139.0074192577352</v>
       </c>
       <c r="C2">
-        <v>0.18153729058697</v>
+        <v>0.2329801838586093</v>
       </c>
       <c r="D2">
-        <v>78.22048605460142</v>
+        <v>156.4241917660677</v>
       </c>
       <c r="E2">
-        <v>0.1998735655173511</v>
+        <v>0.2640757164451414</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -506,16 +587,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>76.27265599568686</v>
+        <v>88.32883758544921</v>
       </c>
       <c r="C3">
-        <v>0.1418879330764435</v>
+        <v>0.1681273413505369</v>
       </c>
       <c r="D3">
-        <v>107.8205008758016</v>
+        <v>99.80065942153301</v>
       </c>
       <c r="E3">
-        <v>0.1617195615870823</v>
+        <v>0.1662667692076085</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -523,16 +604,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>88.94609349568685</v>
+        <v>93.12602640787757</v>
       </c>
       <c r="C4">
-        <v>0.1778064219863028</v>
+        <v>0.1474412957609301</v>
       </c>
       <c r="D4">
-        <v>102.2590905747673</v>
+        <v>118.0655418589266</v>
       </c>
       <c r="E4">
-        <v>0.1872242186563979</v>
+        <v>0.1655199519651886</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -540,67 +621,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>147.7967151006063</v>
+        <v>73.13374226888021</v>
       </c>
       <c r="C5">
-        <v>0.2515338457595408</v>
+        <v>0.1236204713876116</v>
       </c>
       <c r="D5">
-        <v>162.2780245667657</v>
+        <v>79.746022700843</v>
       </c>
       <c r="E5">
-        <v>0.2832247635360615</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>116.2682384570439</v>
-      </c>
-      <c r="C6">
-        <v>0.2454361471042219</v>
-      </c>
-      <c r="D6">
-        <v>122.0560221243291</v>
-      </c>
-      <c r="E6">
-        <v>0.2191548669570894</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>110.6625559488932</v>
-      </c>
-      <c r="C7">
-        <v>0.1808951106031245</v>
-      </c>
-      <c r="D7">
-        <v>127.4876480128168</v>
-      </c>
-      <c r="E7">
-        <v>0.203188924378213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>89.70908762613932</v>
-      </c>
-      <c r="C8">
-        <v>0.1673173655282505</v>
-      </c>
-      <c r="D8">
-        <v>97.36925836864138</v>
-      </c>
-      <c r="E8">
-        <v>0.1527853368696712</v>
+        <v>0.1256463899013074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>